<commit_message>
added multi attachment and attachment gui.
</commit_message>
<xml_diff>
--- a/test.XLSX
+++ b/test.XLSX
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,63 +418,35 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>verma.arpit078@gmail.com</v>
+        <v>blabbla429@gmail.com</v>
       </c>
       <c r="B2" t="str">
-        <v>Arpit</v>
+        <v>bla</v>
       </c>
       <c r="C2" t="str">
-        <v>xyz</v>
+        <v>google</v>
       </c>
       <c r="D2" t="str">
-        <v>23:57 13-06-2023</v>
+        <v>0:43 15-06-2023</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>blabbla429@gmail.com</v>
+        <v>server1078@outlook.com</v>
       </c>
       <c r="B3" t="str">
-        <v>bla</v>
+        <v>server</v>
       </c>
       <c r="C3" t="str">
-        <v>google</v>
+        <v>zerodha</v>
       </c>
       <c r="D3" t="str">
-        <v>23:57 13-06-2023</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2021eeb1156@iitrpr.ac.in</v>
-      </c>
-      <c r="B4" t="str">
-        <v>college id</v>
-      </c>
-      <c r="C4" t="str">
-        <v>oracle</v>
-      </c>
-      <c r="D4" t="str">
-        <v>23:57 13-06-2023</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>server1078@outlook.com</v>
-      </c>
-      <c r="B5" t="str">
-        <v>server</v>
-      </c>
-      <c r="C5" t="str">
-        <v>zerodha</v>
-      </c>
-      <c r="D5" t="str">
-        <v>23:57 13-06-2023</v>
+        <v>0:43 15-06-2023</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
send status on frontend check
</commit_message>
<xml_diff>
--- a/test.XLSX
+++ b/test.XLSX
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,43 +410,86 @@
         <v>Name</v>
       </c>
       <c r="C1" t="str">
-        <v xml:space="preserve">Company </v>
+        <v>Company</v>
       </c>
       <c r="D1" t="str">
+        <v>Message</v>
+      </c>
+      <c r="E1" t="str">
         <v>Sent</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>blabbla429@gmail.com</v>
+        <v>verma.arpit078@gmail.com</v>
       </c>
       <c r="B2" t="str">
-        <v>bla</v>
+        <v>Arpit</v>
       </c>
       <c r="C2" t="str">
-        <v>google</v>
+        <v>Google</v>
       </c>
       <c r="D2" t="str">
-        <v>0:43 15-06-2023</v>
+        <v>Happened to visit your company's website,excited to learn more about this colMail app.</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0:52 18-06-2023</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>2021eeb1156@iitrpr.ac.in</v>
+      </c>
+      <c r="B3" t="str">
+        <v>college</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Google</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Happened to visit your company's website,excited to learn more about this colMail app.</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0:52 18-06-2023</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>blabbla429@gmail.com</v>
+      </c>
+      <c r="B4" t="str">
+        <v>bla</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Google</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Happened to visit your company's website,excited to learn more about this colMail app.</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0:52 18-06-2023</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
         <v>server1078@outlook.com</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B5" t="str">
         <v>server</v>
       </c>
-      <c r="C3" t="str">
-        <v>zerodha</v>
-      </c>
-      <c r="D3" t="str">
-        <v>0:43 15-06-2023</v>
+      <c r="C5" t="str">
+        <v>Google</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Happened to visit your company's website,excited to learn more about this colMail app.</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0:52 18-06-2023</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>